<commit_message>
get the counts of kvp and tables
</commit_message>
<xml_diff>
--- a/interpreter/testFIle.xlsx
+++ b/interpreter/testFIle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-620" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>This is a test excel file</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+  <si>
+    <t>rr</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>tab</t>
+  </si>
+  <si>
+    <t>table</t>
   </si>
 </sst>
 </file>
@@ -57,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,15 +415,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B10:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>